<commit_message>
update the minor change
use explanatory variables with X_data
use dependent variables with y_data
</commit_message>
<xml_diff>
--- a/data/FRED-MD_updated_appendix.xlsx
+++ b/data/FRED-MD_updated_appendix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gredi\Desktop\MADS\696_Milestone2\github\milestoneII\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56638088-A84A-400D-82EC-C3BD090725D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E381D487-80B4-4F77-B5BE-F7FDF6A9DC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3090" yWindow="1305" windowWidth="14670" windowHeight="14175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="0" windowWidth="14700" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FRED-MD_updated_appendix" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3154" uniqueCount="1114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3154" uniqueCount="1115">
   <si>
     <t>id</t>
   </si>
@@ -3598,6 +3598,10 @@
   </si>
   <si>
     <t>tcode</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>WPSFD49207</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -4695,10 +4699,10 @@
   <dimension ref="A1:J224"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D185" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D200" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A224" sqref="A224"/>
+      <selection pane="bottomRight" activeCell="G104" sqref="G104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7282,7 +7286,7 @@
         <v>6</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>375</v>
+        <v>1114</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>376</v>

</xml_diff>